<commit_message>
Office almost done / Soft deleted entities accessibility refactored
</commit_message>
<xml_diff>
--- a/API-List.xlsx
+++ b/API-List.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amir\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\.Programming\.Net\.FullStackCourse\.Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BackOffice-Sale" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="85">
   <si>
     <t>Admin</t>
   </si>
@@ -1687,7 +1687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F3" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -2263,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2379,7 +2379,7 @@
       <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="20" t="s">
         <v>54</v>
       </c>
       <c r="F4" s="13" t="s">
@@ -2415,7 +2415,7 @@
       <c r="C5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="20" t="s">
         <v>55</v>
       </c>
       <c r="F5" s="13" t="s">
@@ -2453,7 +2453,7 @@
       <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="20" t="s">
         <v>60</v>
       </c>
       <c r="F6" s="13"/>
@@ -2477,7 +2477,7 @@
       <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="20" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="13"/>
@@ -2702,8 +2702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2859,7 +2859,9 @@
       <c r="H7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="6"/>
+      <c r="J7" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>

</xml_diff>

<commit_message>
Refactoring IResponse<object> to IResponse / Add "SetModelRequesterId" method to controllers / Change entities access mechanism and remove using OwnerOnly and AdminsOrOwnerOnly policies /  Remove dtos redundant error messages / Remove all "Task.Result"s and replace with "await Task" / Remove User [NationalId,Email,CellPhone] unique constraints due to using those again after soft deleting user
</commit_message>
<xml_diff>
--- a/API-List.xlsx
+++ b/API-List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="BackOffice-Sale" sheetId="4" r:id="rId1"/>
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2702,7 +2702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>